<commit_message>
get diploma image, sample doc
</commit_message>
<xml_diff>
--- a/generator/diplo/data_bachelor_sample.xlsx
+++ b/generator/diplo/data_bachelor_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ediploma\generator\diplo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD8AAE7-6986-4F01-AB28-8FCAF7DCB0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2CBC39-2D95-40AA-9B0D-05F004FAA1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71949462-2A71-4356-B07D-1C6009E12A3E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t>№</t>
   </si>
@@ -72,46 +72,118 @@
     <t>was awarded the degree of bachelor of</t>
   </si>
   <si>
+    <t xml:space="preserve">2023 жылғы 5 маусымдағы №11 хаттама </t>
+  </si>
+  <si>
+    <t xml:space="preserve">от 5 июня 2023, протокол  №11 </t>
+  </si>
+  <si>
+    <t>Dated on June 5, 2023, minute №11</t>
+  </si>
+  <si>
+    <t>Техники и технологий по образовательной программе «6B07101 Химическая технология органических веществ»</t>
+  </si>
+  <si>
+    <t>Степень и квалификация</t>
+  </si>
+  <si>
+    <t>«6B07101 Органикалық заттардың химиялық технологиясы» білім беру бағдарламасы бойынша техника және технология</t>
+  </si>
+  <si>
+    <t>diploma with honours</t>
+  </si>
+  <si>
+    <t>үздік диплом</t>
+  </si>
+  <si>
+    <t>диплом с отличием</t>
+  </si>
+  <si>
+    <t>Engineering and Technology under the Educational programme «6B07101 Chemical Technology of Organic Substances»</t>
+  </si>
+  <si>
+    <t>АО «Казахстанско-Британский технический университет»</t>
+  </si>
+  <si>
     <t>Абухан Ақжол Айдарұлы</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 жылғы 5 маусымдағы №11 хаттама </t>
-  </si>
-  <si>
-    <t xml:space="preserve">от 5 июня 2023, протокол  №11 </t>
-  </si>
-  <si>
-    <t>Dated on June 5, 2023, minute №11</t>
-  </si>
-  <si>
-    <t>Техники и технологий по образовательной программе «6B07101 Химическая технология органических веществ»</t>
-  </si>
-  <si>
-    <t>Степень и квалификация</t>
-  </si>
-  <si>
-    <t>«6B07101 Органикалық заттардың химиялық технологиясы» білім беру бағдарламасы бойынша техника және технология</t>
-  </si>
-  <si>
-    <t>diploma with honours</t>
-  </si>
-  <si>
-    <t>үздік диплом</t>
-  </si>
-  <si>
-    <t>диплом с отличием</t>
-  </si>
-  <si>
     <t>Akzhol Abukhan</t>
   </si>
   <si>
-    <t>Engineering and Technology under the Educational programme «6B07101 Chemical Technology of Organic Substances»</t>
-  </si>
-  <si>
-    <t>Алексей Иванов Сергеевеич</t>
-  </si>
-  <si>
-    <t>Aleksey Ivanov</t>
+    <t>Азаматова Нұрмариям Азаматқызы</t>
+  </si>
+  <si>
+    <t>Nurmariyam Azamatova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 жылғы 5 маусымдағы №1 хаттама </t>
+  </si>
+  <si>
+    <t>от 5 июня 2023, протокол  №1</t>
+  </si>
+  <si>
+    <t>Dated on June 5, 2023, minute №1</t>
+  </si>
+  <si>
+    <t>Айтжанова Айдана Кайратовна</t>
+  </si>
+  <si>
+    <t>Aidana Aitzhanova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 жылғы 6 маусымдағы №12 хаттама </t>
+  </si>
+  <si>
+    <t>от 6 июня 2023, протокол  №12</t>
+  </si>
+  <si>
+    <t>Dated on June 6, 2023, minute №12</t>
+  </si>
+  <si>
+    <t>Аманбаев Мухан Меиримханович</t>
+  </si>
+  <si>
+    <t>Mukhan Amanbayev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 жылғы 6 маусымдағы №15 хаттама </t>
+  </si>
+  <si>
+    <t>от 6 июня 2023, протокол  №15</t>
+  </si>
+  <si>
+    <t>Dated on June 6, 2023, minute №15</t>
+  </si>
+  <si>
+    <t>Аубакиров Даулет Ерикович</t>
+  </si>
+  <si>
+    <t>Daulet Aubakirov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 жылғы 5 маусымдағы №2 хаттама </t>
+  </si>
+  <si>
+    <t>от 5 июня 2023, протокол  №2</t>
+  </si>
+  <si>
+    <t>Dated on June 5, 2023, minute №2</t>
+  </si>
+  <si>
+    <t>Базарбаева Айша Мирлановна</t>
+  </si>
+  <si>
+    <t>Aisha Bazarbayeva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 жылғы 6 маусымдағы №14 хаттама </t>
+  </si>
+  <si>
+    <t>от 6 июня 2023, протокол  №14</t>
+  </si>
+  <si>
+    <t>Dated on June 6, 2023, minute №14</t>
   </si>
 </sst>
 </file>
@@ -220,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -252,9 +324,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -571,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428C3552-F25D-420F-9D46-A39A075DCF74}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -616,7 +685,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -678,106 +747,306 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
     </row>
     <row r="4" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C4" s="6">
         <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>